<commit_message>
excel...causing so much trouble
</commit_message>
<xml_diff>
--- a/src/mongodb/xlsx/data.xlsx
+++ b/src/mongodb/xlsx/data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="548">
   <si>
     <t>ID</t>
   </si>
@@ -1671,6 +1671,9 @@
   </si>
   <si>
     <t>학명_4</t>
+  </si>
+  <si>
+    <t>식품명_5</t>
   </si>
 </sst>
 </file>
@@ -1753,8 +1756,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1784,21 +1789,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2098,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3469,7 +3474,7 @@
   <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3670,519 +3675,898 @@
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="7">
         <v>-4</v>
       </c>
-      <c r="AB2" t="b">
+      <c r="AB2" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="AC2" t="b">
+      <c r="AC2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AD2" t="b">
+      <c r="AD2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="7">
         <v>4.09</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="7">
         <v>2.8</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="7">
         <v>3.3</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="7">
         <v>1</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="7">
         <v>3</v>
       </c>
-      <c r="AK2" t="b">
+      <c r="AK2" s="7" t="b">
         <v>1</v>
       </c>
       <c r="AL2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AM2" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AN2" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AO2" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AP2" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AQ2" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AR2" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AS2" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AU2" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AV2" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="7" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="7">
         <v>-3</v>
       </c>
-      <c r="AB3" t="b">
+      <c r="AB3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AC3" t="b">
+      <c r="AC3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AD3" t="b">
+      <c r="AD3" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="7">
         <v>2.74</v>
       </c>
-      <c r="AH3">
+      <c r="AH3" s="7">
         <v>4.3499999999999996</v>
       </c>
-      <c r="AI3">
+      <c r="AI3" s="7">
         <v>1</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="7">
         <v>5</v>
       </c>
-      <c r="AK3" t="b">
+      <c r="AK3" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="AL3" t="b">
+      <c r="AL3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AM3" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AO3" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AP3" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AQ3" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AR3" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AS3" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AT3" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AU3" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AV3" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AW3" s="7" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Y4" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="7">
         <v>-1</v>
       </c>
-      <c r="AB4" t="b">
+      <c r="AB4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AC4" t="b">
+      <c r="AC4" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="AD4" t="b">
+      <c r="AD4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="7">
         <v>3.08</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="7">
         <v>2.19</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="7">
         <v>2.04</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="7">
         <v>5</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="7">
         <v>5</v>
       </c>
-      <c r="AK4" t="b">
+      <c r="AK4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="AL4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AM4" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AN4" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AO4" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AP4" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="AQ4" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AR4" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AS4" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AT4" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AU4" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AV4" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AW4" s="7" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="7" t="s">
         <v>403</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>-3</v>
+      </c>
+      <c r="AB5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="6">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="AG5" s="6">
+        <v>2.74</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AI5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>5</v>
+      </c>
+      <c r="AK5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="AP5" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AQ5" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="AR5" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="AS5" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="AT5" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="AU5" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="AV5" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="AW5" s="6" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="7" t="s">
         <v>433</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AB6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="6">
+        <v>3.08</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AG6" s="6">
+        <v>2.19</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>2.04</v>
+      </c>
+      <c r="AI6" s="6">
+        <v>5</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AO6" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AP6" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AR6" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AS6" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AT6" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AU6" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AV6" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AW6" s="6" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="7"/>
-      <c r="J7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="AK7" s="1"/>
+      <c r="A7" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="G7" s="7">
+        <v>4</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>-1</v>
+      </c>
+      <c r="AB7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>3.08</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>2.19</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>2.04</v>
+      </c>
+      <c r="AI7" s="6">
+        <v>5</v>
+      </c>
+      <c r="AJ7" s="6">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="AN7" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="AO7" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AP7" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="AQ7" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AR7" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="AS7" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="AT7" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AU7" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="AV7" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="AW7" s="6" t="s">
+        <v>512</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>